<commit_message>
finished data processing for RCs
</commit_message>
<xml_diff>
--- a/data/Max_Stim_PW.xlsx
+++ b/data/Max_Stim_PW.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Channel</t>
   </si>
@@ -77,10 +77,22 @@
     <t>Wrist Flexion, Abduction</t>
   </si>
   <si>
-    <t>wrost flexion</t>
-  </si>
-  <si>
     <t>PW day 2</t>
+  </si>
+  <si>
+    <t>wrist flexion</t>
+  </si>
+  <si>
+    <t>humerus-&gt;wrist</t>
+  </si>
+  <si>
+    <t>humerus-&gt;radius</t>
+  </si>
+  <si>
+    <t>shoulder-&gt;radius</t>
+  </si>
+  <si>
+    <t>humerus-&gt;ulna</t>
   </si>
 </sst>
 </file>
@@ -398,19 +410,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,10 +437,10 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -446,8 +459,11 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -466,8 +482,11 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -486,8 +505,11 @@
       <c r="F4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -506,8 +528,11 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -526,8 +551,11 @@
       <c r="F6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -544,10 +572,13 @@
         <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -563,8 +594,11 @@
       <c r="E8">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -579,6 +613,9 @@
       </c>
       <c r="E9">
         <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding testing data from the lab
</commit_message>
<xml_diff>
--- a/data/Max_Stim_PW.xlsx
+++ b/data/Max_Stim_PW.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Channel</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>humerus-&gt;ulna</t>
+  </si>
+  <si>
+    <t>wrist flexion, abduction</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,6 +424,7 @@
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -594,6 +598,9 @@
       <c r="E8">
         <v>30</v>
       </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" t="s">
         <v>19</v>
       </c>

</xml_diff>